<commit_message>
Final revisions sent to PLOS for production reflected here.
</commit_message>
<xml_diff>
--- a/seriation-analysis/output/pfg-cpl-frequency.xlsx
+++ b/seriation-analysis/output/pfg-cpl-frequency.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="32">
   <si>
     <t>Seriation_Number</t>
   </si>
@@ -441,7 +441,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L204"/>
+  <dimension ref="A1:L206"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1516,22 +1516,22 @@
         <v>28</v>
       </c>
       <c r="B56" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C56">
-        <v>404</v>
+        <v>528</v>
       </c>
       <c r="D56">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="E56">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F56">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G56">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="H56">
         <v>0</v>
@@ -1554,22 +1554,22 @@
         <v>29</v>
       </c>
       <c r="B58" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C58">
-        <v>528</v>
+        <v>404</v>
       </c>
       <c r="D58">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="E58">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G58">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -1592,22 +1592,22 @@
         <v>30</v>
       </c>
       <c r="B60" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C60">
-        <v>404</v>
+        <v>528</v>
       </c>
       <c r="D60">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="E60">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F60">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G60">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -1630,22 +1630,22 @@
         <v>31</v>
       </c>
       <c r="B62" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C62">
-        <v>528</v>
+        <v>404</v>
       </c>
       <c r="D62">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="E62">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G62">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="H62">
         <v>0</v>
@@ -1820,22 +1820,22 @@
         <v>36</v>
       </c>
       <c r="B72" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C72">
-        <v>404</v>
+        <v>764</v>
       </c>
       <c r="D72">
-        <v>208</v>
+        <v>470</v>
       </c>
       <c r="E72">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="F72">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="G72">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -1858,22 +1858,22 @@
         <v>37</v>
       </c>
       <c r="B74" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74">
+        <v>528</v>
+      </c>
+      <c r="D74">
+        <v>198</v>
+      </c>
+      <c r="E74">
+        <v>13</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
         <v>19</v>
-      </c>
-      <c r="C74">
-        <v>764</v>
-      </c>
-      <c r="D74">
-        <v>470</v>
-      </c>
-      <c r="E74">
-        <v>18</v>
-      </c>
-      <c r="F74">
-        <v>5</v>
-      </c>
-      <c r="G74">
-        <v>9</v>
       </c>
       <c r="H74">
         <v>0</v>
@@ -2466,22 +2466,22 @@
         <v>53</v>
       </c>
       <c r="B106" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C106">
-        <v>404</v>
+        <v>528</v>
       </c>
       <c r="D106">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="E106">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F106">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G106">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="H106">
         <v>0</v>
@@ -2504,22 +2504,22 @@
         <v>54</v>
       </c>
       <c r="B108" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C108">
-        <v>528</v>
+        <v>404</v>
       </c>
       <c r="D108">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="E108">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="F108">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G108">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="H108">
         <v>0</v>
@@ -2542,22 +2542,22 @@
         <v>55</v>
       </c>
       <c r="B110" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C110">
-        <v>404</v>
+        <v>528</v>
       </c>
       <c r="D110">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="E110">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F110">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G110">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="H110">
         <v>0</v>
@@ -2580,22 +2580,22 @@
         <v>56</v>
       </c>
       <c r="B112" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C112">
-        <v>528</v>
+        <v>404</v>
       </c>
       <c r="D112">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="E112">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="F112">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G112">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="H112">
         <v>0</v>
@@ -2618,22 +2618,22 @@
         <v>57</v>
       </c>
       <c r="B114" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C114">
-        <v>404</v>
+        <v>528</v>
       </c>
       <c r="D114">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="E114">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F114">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G114">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="H114">
         <v>0</v>
@@ -2656,20 +2656,20 @@
         <v>58</v>
       </c>
       <c r="B116" t="s">
+        <v>21</v>
+      </c>
+      <c r="C116">
+        <v>404</v>
+      </c>
+      <c r="D116">
+        <v>208</v>
+      </c>
+      <c r="E116">
+        <v>6</v>
+      </c>
+      <c r="F116">
         <v>16</v>
       </c>
-      <c r="C116">
-        <v>549</v>
-      </c>
-      <c r="D116">
-        <v>328</v>
-      </c>
-      <c r="E116">
-        <v>77</v>
-      </c>
-      <c r="F116">
-        <v>19</v>
-      </c>
       <c r="G116">
         <v>4</v>
       </c>
@@ -2677,13 +2677,13 @@
         <v>0</v>
       </c>
       <c r="I116">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K116">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L116">
         <v>0</v>
@@ -2694,34 +2694,34 @@
         <v>59</v>
       </c>
       <c r="B118" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C118">
-        <v>865</v>
+        <v>549</v>
       </c>
       <c r="D118">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="E118">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="F118">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G118">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="H118">
         <v>0</v>
       </c>
       <c r="I118">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J118">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K118">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L118">
         <v>0</v>
@@ -2732,22 +2732,22 @@
         <v>60</v>
       </c>
       <c r="B120" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C120">
-        <v>404</v>
+        <v>865</v>
       </c>
       <c r="D120">
-        <v>208</v>
+        <v>323</v>
       </c>
       <c r="E120">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="F120">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G120">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="H120">
         <v>0</v>
@@ -2759,7 +2759,7 @@
         <v>0</v>
       </c>
       <c r="K120">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L120">
         <v>0</v>
@@ -2770,22 +2770,22 @@
         <v>61</v>
       </c>
       <c r="B122" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C122">
-        <v>528</v>
+        <v>404</v>
       </c>
       <c r="D122">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="E122">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="F122">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G122">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="H122">
         <v>0</v>
@@ -2808,22 +2808,22 @@
         <v>62</v>
       </c>
       <c r="B124" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C124">
-        <v>865</v>
+        <v>528</v>
       </c>
       <c r="D124">
-        <v>323</v>
+        <v>198</v>
       </c>
       <c r="E124">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="F124">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="G124">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="H124">
         <v>0</v>
@@ -2835,7 +2835,7 @@
         <v>0</v>
       </c>
       <c r="K124">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L124">
         <v>0</v>
@@ -2846,23 +2846,23 @@
         <v>63</v>
       </c>
       <c r="B126" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C126">
+        <v>865</v>
+      </c>
+      <c r="D126">
+        <v>323</v>
+      </c>
+      <c r="E126">
+        <v>59</v>
+      </c>
+      <c r="F126">
+        <v>17</v>
+      </c>
+      <c r="G126">
         <v>35</v>
       </c>
-      <c r="D126">
-        <v>11</v>
-      </c>
-      <c r="E126">
-        <v>33</v>
-      </c>
-      <c r="F126">
-        <v>0</v>
-      </c>
-      <c r="G126">
-        <v>0</v>
-      </c>
       <c r="H126">
         <v>0</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>0</v>
       </c>
       <c r="K126">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L126">
         <v>0</v>
@@ -2884,22 +2884,22 @@
         <v>64</v>
       </c>
       <c r="B128" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C128">
-        <v>528</v>
+        <v>35</v>
       </c>
       <c r="D128">
-        <v>198</v>
+        <v>11</v>
       </c>
       <c r="E128">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="F128">
         <v>0</v>
       </c>
       <c r="G128">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="H128">
         <v>0</v>
@@ -2922,22 +2922,22 @@
         <v>65</v>
       </c>
       <c r="B130" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C130">
-        <v>404</v>
+        <v>528</v>
       </c>
       <c r="D130">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="E130">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F130">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G130">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="H130">
         <v>0</v>
@@ -2960,22 +2960,22 @@
         <v>66</v>
       </c>
       <c r="B132" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C132">
-        <v>865</v>
+        <v>404</v>
       </c>
       <c r="D132">
-        <v>323</v>
+        <v>208</v>
       </c>
       <c r="E132">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="F132">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G132">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="H132">
         <v>0</v>
@@ -2987,7 +2987,7 @@
         <v>0</v>
       </c>
       <c r="K132">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L132">
         <v>0</v>
@@ -2998,22 +2998,22 @@
         <v>67</v>
       </c>
       <c r="B134" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C134">
-        <v>764</v>
+        <v>865</v>
       </c>
       <c r="D134">
-        <v>470</v>
+        <v>323</v>
       </c>
       <c r="E134">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="F134">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="G134">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="H134">
         <v>0</v>
@@ -3025,7 +3025,7 @@
         <v>0</v>
       </c>
       <c r="K134">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L134">
         <v>0</v>
@@ -3036,22 +3036,22 @@
         <v>68</v>
       </c>
       <c r="B136" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C136">
-        <v>528</v>
+        <v>764</v>
       </c>
       <c r="D136">
-        <v>198</v>
+        <v>470</v>
       </c>
       <c r="E136">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F136">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G136">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="H136">
         <v>0</v>
@@ -3074,37 +3074,37 @@
         <v>69</v>
       </c>
       <c r="B138" t="s">
+        <v>23</v>
+      </c>
+      <c r="C138">
+        <v>244</v>
+      </c>
+      <c r="D138">
+        <v>40</v>
+      </c>
+      <c r="E138">
+        <v>18</v>
+      </c>
+      <c r="F138">
+        <v>1</v>
+      </c>
+      <c r="G138">
+        <v>16</v>
+      </c>
+      <c r="H138">
+        <v>21</v>
+      </c>
+      <c r="I138">
+        <v>0</v>
+      </c>
+      <c r="J138">
         <v>14</v>
       </c>
-      <c r="C138">
-        <v>528</v>
-      </c>
-      <c r="D138">
-        <v>198</v>
-      </c>
-      <c r="E138">
-        <v>13</v>
-      </c>
-      <c r="F138">
-        <v>0</v>
-      </c>
-      <c r="G138">
-        <v>19</v>
-      </c>
-      <c r="H138">
-        <v>0</v>
-      </c>
-      <c r="I138">
-        <v>0</v>
-      </c>
-      <c r="J138">
-        <v>0</v>
-      </c>
       <c r="K138">
         <v>0</v>
       </c>
       <c r="L138">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="140" spans="1:12">
@@ -3112,22 +3112,22 @@
         <v>70</v>
       </c>
       <c r="B140" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C140">
-        <v>404</v>
+        <v>528</v>
       </c>
       <c r="D140">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="E140">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F140">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G140">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="H140">
         <v>0</v>
@@ -3226,34 +3226,34 @@
         <v>73</v>
       </c>
       <c r="B146" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C146">
-        <v>549</v>
+        <v>528</v>
       </c>
       <c r="D146">
-        <v>328</v>
+        <v>198</v>
       </c>
       <c r="E146">
-        <v>77</v>
+        <v>13</v>
       </c>
       <c r="F146">
+        <v>0</v>
+      </c>
+      <c r="G146">
         <v>19</v>
       </c>
-      <c r="G146">
-        <v>4</v>
-      </c>
       <c r="H146">
         <v>0</v>
       </c>
       <c r="I146">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J146">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K146">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L146">
         <v>0</v>
@@ -3264,22 +3264,22 @@
         <v>74</v>
       </c>
       <c r="B148" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C148">
-        <v>865</v>
+        <v>404</v>
       </c>
       <c r="D148">
-        <v>323</v>
+        <v>208</v>
       </c>
       <c r="E148">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="F148">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G148">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="H148">
         <v>0</v>
@@ -3291,7 +3291,7 @@
         <v>0</v>
       </c>
       <c r="K148">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L148">
         <v>0</v>
@@ -3302,19 +3302,19 @@
         <v>75</v>
       </c>
       <c r="B150" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C150">
-        <v>404</v>
+        <v>549</v>
       </c>
       <c r="D150">
-        <v>208</v>
+        <v>328</v>
       </c>
       <c r="E150">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="F150">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G150">
         <v>4</v>
@@ -3323,13 +3323,13 @@
         <v>0</v>
       </c>
       <c r="I150">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J150">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K150">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L150">
         <v>0</v>
@@ -3340,22 +3340,22 @@
         <v>76</v>
       </c>
       <c r="B152" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C152">
-        <v>528</v>
+        <v>865</v>
       </c>
       <c r="D152">
-        <v>198</v>
+        <v>323</v>
       </c>
       <c r="E152">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="F152">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G152">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="H152">
         <v>0</v>
@@ -3367,7 +3367,7 @@
         <v>0</v>
       </c>
       <c r="K152">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L152">
         <v>0</v>
@@ -3378,22 +3378,22 @@
         <v>77</v>
       </c>
       <c r="B154" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C154">
-        <v>865</v>
+        <v>404</v>
       </c>
       <c r="D154">
-        <v>323</v>
+        <v>208</v>
       </c>
       <c r="E154">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="F154">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G154">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="H154">
         <v>0</v>
@@ -3405,7 +3405,7 @@
         <v>0</v>
       </c>
       <c r="K154">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L154">
         <v>0</v>
@@ -3416,22 +3416,22 @@
         <v>78</v>
       </c>
       <c r="B156" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C156">
-        <v>35</v>
+        <v>528</v>
       </c>
       <c r="D156">
-        <v>11</v>
+        <v>198</v>
       </c>
       <c r="E156">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="F156">
         <v>0</v>
       </c>
       <c r="G156">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="H156">
         <v>0</v>
@@ -3454,22 +3454,22 @@
         <v>79</v>
       </c>
       <c r="B158" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C158">
-        <v>528</v>
+        <v>865</v>
       </c>
       <c r="D158">
-        <v>198</v>
+        <v>323</v>
       </c>
       <c r="E158">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="F158">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G158">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="H158">
         <v>0</v>
@@ -3481,7 +3481,7 @@
         <v>0</v>
       </c>
       <c r="K158">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L158">
         <v>0</v>
@@ -3492,22 +3492,22 @@
         <v>80</v>
       </c>
       <c r="B160" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C160">
-        <v>404</v>
+        <v>35</v>
       </c>
       <c r="D160">
-        <v>208</v>
+        <v>11</v>
       </c>
       <c r="E160">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="F160">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G160">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H160">
         <v>0</v>
@@ -3530,22 +3530,22 @@
         <v>81</v>
       </c>
       <c r="B162" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C162">
-        <v>865</v>
+        <v>528</v>
       </c>
       <c r="D162">
-        <v>323</v>
+        <v>198</v>
       </c>
       <c r="E162">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="F162">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="G162">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="H162">
         <v>0</v>
@@ -3557,7 +3557,7 @@
         <v>0</v>
       </c>
       <c r="K162">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L162">
         <v>0</v>
@@ -3568,22 +3568,22 @@
         <v>82</v>
       </c>
       <c r="B164" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C164">
-        <v>764</v>
+        <v>404</v>
       </c>
       <c r="D164">
-        <v>470</v>
+        <v>208</v>
       </c>
       <c r="E164">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="F164">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="G164">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H164">
         <v>0</v>
@@ -3606,22 +3606,22 @@
         <v>83</v>
       </c>
       <c r="B166" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C166">
-        <v>528</v>
+        <v>865</v>
       </c>
       <c r="D166">
-        <v>198</v>
+        <v>323</v>
       </c>
       <c r="E166">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="F166">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G166">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="H166">
         <v>0</v>
@@ -3633,7 +3633,7 @@
         <v>0</v>
       </c>
       <c r="K166">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L166">
         <v>0</v>
@@ -3644,22 +3644,22 @@
         <v>84</v>
       </c>
       <c r="B168" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C168">
-        <v>404</v>
+        <v>764</v>
       </c>
       <c r="D168">
-        <v>208</v>
+        <v>470</v>
       </c>
       <c r="E168">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="F168">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="G168">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H168">
         <v>0</v>
@@ -3682,22 +3682,22 @@
         <v>85</v>
       </c>
       <c r="B170" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C170">
-        <v>404</v>
+        <v>528</v>
       </c>
       <c r="D170">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="E170">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F170">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G170">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="H170">
         <v>0</v>
@@ -3758,20 +3758,20 @@
         <v>87</v>
       </c>
       <c r="B174" t="s">
+        <v>21</v>
+      </c>
+      <c r="C174">
+        <v>404</v>
+      </c>
+      <c r="D174">
+        <v>208</v>
+      </c>
+      <c r="E174">
+        <v>6</v>
+      </c>
+      <c r="F174">
         <v>16</v>
       </c>
-      <c r="C174">
-        <v>549</v>
-      </c>
-      <c r="D174">
-        <v>328</v>
-      </c>
-      <c r="E174">
-        <v>77</v>
-      </c>
-      <c r="F174">
-        <v>19</v>
-      </c>
       <c r="G174">
         <v>4</v>
       </c>
@@ -3779,13 +3779,13 @@
         <v>0</v>
       </c>
       <c r="I174">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J174">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K174">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L174">
         <v>0</v>
@@ -3834,19 +3834,19 @@
         <v>89</v>
       </c>
       <c r="B178" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C178">
-        <v>404</v>
+        <v>549</v>
       </c>
       <c r="D178">
-        <v>208</v>
+        <v>328</v>
       </c>
       <c r="E178">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="F178">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G178">
         <v>4</v>
@@ -3855,13 +3855,13 @@
         <v>0</v>
       </c>
       <c r="I178">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J178">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K178">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L178">
         <v>0</v>
@@ -3872,22 +3872,22 @@
         <v>90</v>
       </c>
       <c r="B180" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C180">
-        <v>764</v>
+        <v>404</v>
       </c>
       <c r="D180">
-        <v>470</v>
+        <v>208</v>
       </c>
       <c r="E180">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="F180">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="G180">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H180">
         <v>0</v>
@@ -3948,22 +3948,22 @@
         <v>92</v>
       </c>
       <c r="B184" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C184">
-        <v>39</v>
+        <v>764</v>
       </c>
       <c r="D184">
-        <v>62</v>
+        <v>470</v>
       </c>
       <c r="E184">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F184">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G184">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H184">
         <v>0</v>
@@ -3978,7 +3978,7 @@
         <v>0</v>
       </c>
       <c r="L184">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="186" spans="1:12">
@@ -3986,22 +3986,22 @@
         <v>93</v>
       </c>
       <c r="B186" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C186">
-        <v>39</v>
+        <v>404</v>
       </c>
       <c r="D186">
-        <v>62</v>
+        <v>208</v>
       </c>
       <c r="E186">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="F186">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G186">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H186">
         <v>0</v>
@@ -4016,7 +4016,7 @@
         <v>0</v>
       </c>
       <c r="L186">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="188" spans="1:12">
@@ -4062,37 +4062,37 @@
         <v>95</v>
       </c>
       <c r="B190" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C190">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="D190">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="E190">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="F190">
         <v>0</v>
       </c>
       <c r="G190">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H190">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I190">
         <v>0</v>
       </c>
       <c r="J190">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K190">
         <v>0</v>
       </c>
       <c r="L190">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="192" spans="1:12">
@@ -4100,16 +4100,16 @@
         <v>96</v>
       </c>
       <c r="B192" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C192">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D192">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="E192">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="F192">
         <v>0</v>
@@ -4130,7 +4130,7 @@
         <v>0</v>
       </c>
       <c r="L192">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="194" spans="1:12">
@@ -4138,31 +4138,31 @@
         <v>97</v>
       </c>
       <c r="B194" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C194">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D194">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="E194">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="F194">
         <v>0</v>
       </c>
       <c r="G194">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H194">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I194">
         <v>0</v>
       </c>
       <c r="J194">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K194">
         <v>0</v>
@@ -4176,16 +4176,16 @@
         <v>98</v>
       </c>
       <c r="B196" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C196">
         <v>35</v>
       </c>
       <c r="D196">
-        <v>65</v>
+        <v>11</v>
       </c>
       <c r="E196">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="F196">
         <v>0</v>
@@ -4194,19 +4194,19 @@
         <v>0</v>
       </c>
       <c r="H196">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I196">
         <v>0</v>
       </c>
       <c r="J196">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K196">
         <v>0</v>
       </c>
       <c r="L196">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="198" spans="1:12">
@@ -4214,25 +4214,25 @@
         <v>99</v>
       </c>
       <c r="B198" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C198">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="D198">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="E198">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="F198">
         <v>0</v>
       </c>
       <c r="G198">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H198">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I198">
         <v>0</v>
@@ -4252,37 +4252,37 @@
         <v>100</v>
       </c>
       <c r="B200" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C200">
-        <v>528</v>
+        <v>35</v>
       </c>
       <c r="D200">
-        <v>198</v>
+        <v>65</v>
       </c>
       <c r="E200">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F200">
         <v>0</v>
       </c>
       <c r="G200">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="H200">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I200">
         <v>0</v>
       </c>
       <c r="J200">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K200">
         <v>0</v>
       </c>
       <c r="L200">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202" spans="1:12">
@@ -4290,25 +4290,25 @@
         <v>101</v>
       </c>
       <c r="B202" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C202">
-        <v>404</v>
+        <v>42</v>
       </c>
       <c r="D202">
-        <v>208</v>
+        <v>56</v>
       </c>
       <c r="E202">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="F202">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G202">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H202">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I202">
         <v>0</v>
@@ -4328,22 +4328,22 @@
         <v>102</v>
       </c>
       <c r="B204" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C204">
-        <v>35</v>
+        <v>528</v>
       </c>
       <c r="D204">
-        <v>11</v>
+        <v>198</v>
       </c>
       <c r="E204">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="F204">
         <v>0</v>
       </c>
       <c r="G204">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="H204">
         <v>0</v>
@@ -4358,6 +4358,44 @@
         <v>0</v>
       </c>
       <c r="L204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12">
+      <c r="A206">
+        <v>103</v>
+      </c>
+      <c r="B206" t="s">
+        <v>21</v>
+      </c>
+      <c r="C206">
+        <v>404</v>
+      </c>
+      <c r="D206">
+        <v>208</v>
+      </c>
+      <c r="E206">
+        <v>6</v>
+      </c>
+      <c r="F206">
+        <v>16</v>
+      </c>
+      <c r="G206">
+        <v>4</v>
+      </c>
+      <c r="H206">
+        <v>0</v>
+      </c>
+      <c r="I206">
+        <v>0</v>
+      </c>
+      <c r="J206">
+        <v>0</v>
+      </c>
+      <c r="K206">
+        <v>0</v>
+      </c>
+      <c r="L206">
         <v>0</v>
       </c>
     </row>

</xml_diff>